<commit_message>
documentation and BERT results
</commit_message>
<xml_diff>
--- a/informes/Gantt_Implementacio.xlsx
+++ b/informes/Gantt_Implementacio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcaix\UAB\TFG\informes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65AC8A0A-4063-4748-8C64-2DEB11E58664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39C9F6A-7DA8-40E3-A0C3-E4F540DD250D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12195" yWindow="5415" windowWidth="25425" windowHeight="14685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5130" yWindow="2625" windowWidth="25425" windowHeight="14685" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Planificació realitzada" sheetId="6" r:id="rId1"/>
@@ -2952,7 +2952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD4C9665-836D-41AD-8A57-A46768844E4A}">
   <dimension ref="A1:V64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:V64"/>
     </sheetView>
   </sheetViews>
@@ -3873,7 +3873,7 @@
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="15"/>
-      <c r="I35" s="20"/>
+      <c r="I35" s="40"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
@@ -3899,9 +3899,9 @@
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="15"/>
-      <c r="I36" s="24"/>
+      <c r="I36" s="52"/>
       <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
+      <c r="K36" s="50"/>
       <c r="L36" s="1"/>
       <c r="M36" s="1"/>
       <c r="N36" s="1"/>
@@ -3925,9 +3925,9 @@
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="15"/>
-      <c r="I37" s="24"/>
-      <c r="J37" s="24"/>
-      <c r="K37" s="1"/>
+      <c r="I37" s="52"/>
+      <c r="J37" s="52"/>
+      <c r="K37" s="50"/>
       <c r="L37" s="1"/>
       <c r="M37" s="1"/>
       <c r="N37" s="1"/>
@@ -3951,10 +3951,10 @@
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="15"/>
-      <c r="I38" s="24"/>
+      <c r="I38" s="52"/>
       <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1"/>
+      <c r="K38" s="50"/>
+      <c r="L38" s="50"/>
       <c r="M38" s="1"/>
       <c r="N38" s="1"/>
       <c r="O38" s="1"/>
@@ -3978,9 +3978,9 @@
       <c r="G39" s="1"/>
       <c r="H39" s="15"/>
       <c r="I39" s="1"/>
-      <c r="J39" s="24"/>
+      <c r="J39" s="52"/>
       <c r="K39" s="1"/>
-      <c r="L39" s="1"/>
+      <c r="L39" s="50"/>
       <c r="M39" s="1"/>
       <c r="N39" s="1"/>
       <c r="O39" s="1"/>
@@ -4003,11 +4003,11 @@
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
       <c r="H40" s="15"/>
-      <c r="I40" s="24"/>
-      <c r="J40" s="24"/>
-      <c r="K40" s="24"/>
-      <c r="L40" s="24"/>
-      <c r="M40" s="24"/>
+      <c r="I40" s="52"/>
+      <c r="J40" s="52"/>
+      <c r="K40" s="52"/>
+      <c r="L40" s="40"/>
+      <c r="M40" s="40"/>
       <c r="N40" s="1"/>
       <c r="O40" s="1"/>
       <c r="P40" s="1"/>
@@ -4031,9 +4031,9 @@
       <c r="H41" s="15"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
-      <c r="K41" s="24"/>
-      <c r="L41" s="24"/>
-      <c r="M41" s="24"/>
+      <c r="K41" s="52"/>
+      <c r="L41" s="52"/>
+      <c r="M41" s="50"/>
       <c r="N41" s="1"/>
       <c r="O41" s="1"/>
       <c r="P41" s="1"/>
@@ -4057,7 +4057,7 @@
       <c r="H42" s="15"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
-      <c r="K42" s="24"/>
+      <c r="K42" s="52"/>
       <c r="L42" s="1"/>
       <c r="M42" s="1"/>
       <c r="N42" s="1"/>
@@ -4084,8 +4084,8 @@
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
-      <c r="L43" s="24"/>
-      <c r="M43" s="1"/>
+      <c r="L43" s="52"/>
+      <c r="M43" s="50"/>
       <c r="N43" s="1"/>
       <c r="O43" s="1"/>
       <c r="P43" s="1"/>
@@ -4111,7 +4111,7 @@
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
-      <c r="M44" s="24"/>
+      <c r="M44" s="50"/>
       <c r="N44" s="1"/>
       <c r="O44" s="1"/>
       <c r="P44" s="1"/>

</xml_diff>